<commit_message>
Addition of flat-run technologies (CHP)
</commit_message>
<xml_diff>
--- a/Input Data/Generator_efficiencies.xlsx
+++ b/Input Data/Generator_efficiencies.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15" conformance="strict">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr dateCompatibility="0" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0138303\Documents\DispatchModelEU\Input Data\"/>
@@ -17,8 +17,11 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$17</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="162913"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="23" uniqueCount="23">
   <si>
     <t>CCGT</t>
   </si>
@@ -101,7 +104,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -121,8 +124,8 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -152,7 +155,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -271,25 +274,25 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:lumMod val="110%"/>
+                <a:satMod val="105%"/>
+                <a:tint val="67%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:lumMod val="105%"/>
+                <a:satMod val="103%"/>
+                <a:tint val="73%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:lumMod val="105%"/>
+                <a:satMod val="109%"/>
+                <a:tint val="81%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -297,25 +300,25 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:satMod val="103%"/>
+                <a:lumMod val="102%"/>
+                <a:tint val="94%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:satMod val="110%"/>
+                <a:lumMod val="100%"/>
+                <a:shade val="100%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:lumMod val="99%"/>
+                <a:satMod val="120%"/>
+                <a:shade val="78%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -328,21 +331,21 @@
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -356,7 +359,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="63%"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -368,32 +371,32 @@
         </a:solidFill>
         <a:solidFill>
           <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
+            <a:tint val="95%"/>
+            <a:satMod val="170%"/>
           </a:schemeClr>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="93%"/>
+                <a:satMod val="150%"/>
+                <a:shade val="98%"/>
+                <a:lumMod val="102%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="98%"/>
+                <a:satMod val="130%"/>
+                <a:shade val="90%"/>
+                <a:lumMod val="103%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="63%"/>
+                <a:satMod val="120%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -413,21 +416,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -450,7 +453,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -464,7 +467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -488,7 +491,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -512,7 +515,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -536,7 +539,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -560,7 +563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -584,7 +587,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -608,7 +611,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -632,7 +635,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -656,7 +659,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -674,7 +677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -692,7 +695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -707,7 +710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -725,7 +728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -743,7 +746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -758,7 +761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -773,31 +776,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
     </row>
   </sheetData>

</xml_diff>